<commit_message>
working on different parameters for snakes
</commit_message>
<xml_diff>
--- a/figs/activeContour_dec17/summary/PVE_active_contours.xlsx
+++ b/figs/activeContour_dec17/summary/PVE_active_contours.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="44">
   <si>
     <t xml:space="preserve">Edges</t>
   </si>
@@ -147,6 +148,12 @@
   </si>
   <si>
     <t xml:space="preserve">Seg 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snakes – 2412-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snakes – 2412-02</t>
   </si>
 </sst>
 </file>
@@ -361,14 +368,14 @@
   </sheetPr>
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,13 +2616,13 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3087,4 +3094,668 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.9897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>52295.681</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>25264.893</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>22822.453</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>25799.604</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>50882.94</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">AVERAGE(B2:F2)</f>
+        <v>35413.1142</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">MAX(B2:F2)</f>
+        <v>52295.681</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">MIN(B2:F2)</f>
+        <v>22822.453</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>49914.849</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>23469.238</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>20752.461</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>24804.792</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>47637.539</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">AVERAGE(B3:F3)</f>
+        <v>33315.7758</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">MAX(B3:F3)</f>
+        <v>49914.849</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">MIN(B3:F3)</f>
+        <v>20752.461</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false">AVERAGE(B4:F4)</f>
+        <v>0.0622</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <f aca="false">MAX(B4:F4)</f>
+        <v>0.091</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <f aca="false">MIN(B4:F4)</f>
+        <v>0.039</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>32805.908</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9591.064</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>11771.3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>15589.534</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>34140.034</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">AVERAGE(B5:F5)</f>
+        <v>20779.568</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">MAX(B5:F5)</f>
+        <v>34140.034</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">MIN(B5:F5)</f>
+        <v>9591.064</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>35978.927</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>15380.249</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>14265.971</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>19350.482</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>40749.531</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">AVERAGE(B6:F6)</f>
+        <v>25145.032</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">MAX(B6:F6)</f>
+        <v>40749.531</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">MIN(B6:F6)</f>
+        <v>14265.971</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>-0.097</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>-0.604</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>-0.212</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <f aca="false">-0.241</f>
+        <v>-0.241</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>-0.194</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <f aca="false">AVERAGE(B7:F7)</f>
+        <v>-0.2696</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <f aca="false">MAX(B7:F7)</f>
+        <v>-0.097</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <f aca="false">MIN(B7:F7)</f>
+        <v>-0.604</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>19489.773</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>15673.828</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>11051.153</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>10210.069</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>16742.907</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">AVERAGE(B8:F8)</f>
+        <v>14633.546</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">MAX(B8:F8)</f>
+        <v>19489.773</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">MIN(B8:F8)</f>
+        <v>10210.069</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>13935.921</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>8088.989</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>6486.49</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>5454.31</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>6888.008</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">AVERAGE(B9:F9)</f>
+        <v>8170.7436</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">MAX(B9:F9)</f>
+        <v>13935.921</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">MIN(B9:F9)</f>
+        <v>5454.31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>0.285</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0.466</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0.589</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <f aca="false">AVERAGE(B10:F10)</f>
+        <v>0.4474</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <f aca="false">MAX(B10:F10)</f>
+        <v>0.589</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <f aca="false">MIN(B10:F10)</f>
+        <v>0.285</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>52295.681</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>25264.893</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>22822.453</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>25799.604</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>50882.94</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">AVERAGE(B14:F14)</f>
+        <v>35413.1142</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">MAX(B14:F14)</f>
+        <v>52295.681</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">MIN(B14:F14)</f>
+        <v>22822.453</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>49927.672</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>23166.504</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>20624.11</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>24829.741</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>47423.983</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">AVERAGE(B15:F15)</f>
+        <v>33194.402</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">MAX(B15:F15)</f>
+        <v>49927.672</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">MIN(B15:F15)</f>
+        <v>20624.11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <f aca="false">AVERAGE(B16:F16)</f>
+        <v>0.066</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <f aca="false">MAX(B16:F16)</f>
+        <v>0.096</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <f aca="false">MIN(B16:F16)</f>
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>32805.908</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>9591.064</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>11771.3</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>15589.534</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>34140.034</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">AVERAGE(B17:F17)</f>
+        <v>20779.568</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">MAX(B17:F17)</f>
+        <v>34140.034</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">MIN(B17:F17)</f>
+        <v>9591.064</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>29906.45</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>13271.484</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>11724.783</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>16094.736</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>37310.2</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">AVERAGE(B18:F18)</f>
+        <v>21661.5306</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">MAX(B18:F18)</f>
+        <v>37310.2</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">MIN(B18:F18)</f>
+        <v>11724.783</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>0.088</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>-0.384</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <f aca="false">-0.032</f>
+        <v>-0.032</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>-0.093</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">AVERAGE(B19:F19)</f>
+        <v>-0.0834</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <f aca="false">MAX(B19:F19)</f>
+        <v>0.088</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <f aca="false">MIN(B19:F19)</f>
+        <v>-0.384</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>19489.773</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>15673.828</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>11051.153</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>10210.069</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>16742.907</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">AVERAGE(B20:F20)</f>
+        <v>14633.546</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">MAX(B20:F20)</f>
+        <v>19489.773</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">MIN(B20:F20)</f>
+        <v>10210.069</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>20021.221</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>9895.02</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>8899.327</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>8735.004</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>10113.783</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">AVERAGE(B21:F21)</f>
+        <v>11532.871</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">MAX(B21:F21)</f>
+        <v>20021.221</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">MIN(B21:F21)</f>
+        <v>8735.004</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>-0.027</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>0.369</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <f aca="false">AVERAGE(B22:F22)</f>
+        <v>0.2154</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <f aca="false">MAX(B22:F22)</f>
+        <v>0.396</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <f aca="false">MIN(B22:F22)</f>
+        <v>-0.027</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>